<commit_message>
changes to excel to stash
</commit_message>
<xml_diff>
--- a/LandRegistryProject/TestDatas/TittleNumer.xlsx
+++ b/LandRegistryProject/TestDatas/TittleNumer.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HomesEnglandAutomation\Land_Registry\LandRegistryProject\TestDatas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amos.Awaghade\source\repos\LandRegistryBulk-Discharge-Automation\LandRegistryProject\TestDatas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B4AC233-91E9-424C-97B3-A7843E71FA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AE6B8E-D7D9-4413-8E49-EF1CCCEA3EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="910" yWindow="0" windowWidth="22380" windowHeight="11270" xr2:uid="{BA3442DB-404F-46D9-B4F8-C3AAD76398EE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BA3442DB-404F-46D9-B4F8-C3AAD76398EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,62 +38,56 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
+    <t>30 Wallace Green Way, Walkern, Stevenage (SG2 7FB)</t>
+  </si>
+  <si>
+    <t>Hg545432</t>
+  </si>
+  <si>
+    <t>32 Wallace Green Way, Walkern, Stevenage (SG2 7FB)</t>
+  </si>
+  <si>
+    <t>HD602385</t>
+  </si>
+  <si>
+    <t>WT99999/BBB5555/190</t>
+  </si>
+  <si>
+    <t>Submitted</t>
+  </si>
+  <si>
+    <t>33 Wallace Green Way, Walkern, Stevenage (SG2 7FB)</t>
+  </si>
+  <si>
+    <t>HD602386</t>
+  </si>
+  <si>
+    <t>WT99999/TTr5555/190</t>
+  </si>
+  <si>
+    <t>34 Wallace Green Way, Walkern, Stevenage (SG2 7FB)</t>
+  </si>
+  <si>
+    <t>HD602387</t>
+  </si>
+  <si>
+    <t>WT99999/YYr5555/190</t>
+  </si>
+  <si>
+    <t>31 Wallace Green Way, Walkern, Stevenage (SG2 7FB)</t>
+  </si>
+  <si>
     <t>HD602384</t>
-  </si>
-  <si>
-    <t>HD602385</t>
-  </si>
-  <si>
-    <t>HD602386</t>
-  </si>
-  <si>
-    <t>HD602387</t>
-  </si>
-  <si>
-    <t>Submitted</t>
-  </si>
-  <si>
-    <t>WT99999/TTr5555/190</t>
-  </si>
-  <si>
-    <t>WT99999/YYr5555/190</t>
-  </si>
-  <si>
-    <t>WT99999/BBB5555/190</t>
-  </si>
-  <si>
-    <t>Hg545432</t>
-  </si>
-  <si>
-    <t>31 Wallace Green Way, Walkern, Stevenage (SG2 7FB)</t>
-  </si>
-  <si>
-    <t>32 Wallace Green Way, Walkern, Stevenage (SG2 7FB)</t>
-  </si>
-  <si>
-    <t>33 Wallace Green Way, Walkern, Stevenage (SG2 7FB)</t>
-  </si>
-  <si>
-    <t>34 Wallace Green Way, Walkern, Stevenage (SG2 7FB)</t>
-  </si>
-  <si>
-    <t>30 Wallace Green Way, Walkern, Stevenage (SG2 7FB)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -139,9 +133,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -179,7 +173,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -285,7 +279,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -427,7 +421,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -437,103 +431,103 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB411934-2E25-4BF9-A7BD-3E1F9CE09557}">
   <dimension ref="D1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="52.1796875" customWidth="1"/>
-    <col min="5" max="5" width="18.7265625" customWidth="1"/>
+    <col min="4" max="4" width="52.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="45.81640625" customWidth="1"/>
+    <col min="10" max="10" width="45.85546875" customWidth="1"/>
     <col min="11" max="11" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E1">
         <v>33333</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="4:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>55556</v>
       </c>
       <c r="I2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="K2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="M2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="4:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E3">
         <v>55557</v>
       </c>
       <c r="I3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="K3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" t="s">
         <v>5</v>
       </c>
-      <c r="M3" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="4" spans="4:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E4">
         <v>55558</v>
       </c>
       <c r="I4" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="J4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
         <v>12</v>
-      </c>
-      <c r="K4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="4:13" x14ac:dyDescent="0.35">
-      <c r="D5" t="s">
-        <v>9</v>
       </c>
       <c r="E5">
         <v>55555</v>
       </c>
       <c r="I5" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;12&amp;K0078D7 OFFICIAL </oddFooter>

</xml_diff>

<commit_message>
complete loop through sheet
</commit_message>
<xml_diff>
--- a/LandRegistryProject/TestDatas/TittleNumer.xlsx
+++ b/LandRegistryProject/TestDatas/TittleNumer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amos.Awaghade\source\repos\LandRegistryBulk-Discharge-Automation\LandRegistryProject\TestDatas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AE6B8E-D7D9-4413-8E49-EF1CCCEA3EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FEC6FD-35C0-4E7D-B03D-BBAB69F0691F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BA3442DB-404F-46D9-B4F8-C3AAD76398EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>30 Wallace Green Way, Walkern, Stevenage (SG2 7FB)</t>
   </si>
@@ -44,16 +44,19 @@
     <t>Hg545432</t>
   </si>
   <si>
-    <t>32 Wallace Green Way, Walkern, Stevenage (SG2 7FB)</t>
+    <t>Submitted</t>
+  </si>
+  <si>
+    <t>Vineyard Barn, The Vineyard, Welwyn Garden City (AL8 7PU)</t>
   </si>
   <si>
     <t>HD602385</t>
   </si>
   <si>
-    <t>WT99999/BBB5555/190</t>
-  </si>
-  <si>
-    <t>Submitted</t>
+    <t>31 Wallace Green Way, Walkern, Stevenage (SG2 7FB)</t>
+  </si>
+  <si>
+    <t>HD602384</t>
   </si>
   <si>
     <t>33 Wallace Green Way, Walkern, Stevenage (SG2 7FB)</t>
@@ -62,22 +65,10 @@
     <t>HD602386</t>
   </si>
   <si>
-    <t>WT99999/TTr5555/190</t>
-  </si>
-  <si>
     <t>34 Wallace Green Way, Walkern, Stevenage (SG2 7FB)</t>
   </si>
   <si>
     <t>HD602387</t>
-  </si>
-  <si>
-    <t>WT99999/YYr5555/190</t>
-  </si>
-  <si>
-    <t>31 Wallace Green Way, Walkern, Stevenage (SG2 7FB)</t>
-  </si>
-  <si>
-    <t>HD602384</t>
   </si>
 </sst>
 </file>
@@ -429,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB411934-2E25-4BF9-A7BD-3E1F9CE09557}">
-  <dimension ref="D1:M5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +435,10 @@
     <col min="11" max="11" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
@@ -454,76 +448,87 @@
       <c r="I1" t="s">
         <v>1</v>
       </c>
+      <c r="M1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2">
         <v>55556</v>
       </c>
       <c r="I2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>3</v>
       </c>
-      <c r="J2" t="s">
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>55555</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>55557</v>
+      </c>
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" t="s">
         <v>2</v>
       </c>
-      <c r="K2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" t="s">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>5</v>
       </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>55558</v>
+      </c>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>6</v>
       </c>
-      <c r="E3">
-        <v>55557</v>
-      </c>
-      <c r="I3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>55555</v>
+      </c>
+      <c r="I6" t="s">
         <v>6</v>
-      </c>
-      <c r="K3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4">
-        <v>55558</v>
-      </c>
-      <c r="I4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5">
-        <v>55555</v>
-      </c>
-      <c r="I5" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes made in validate fields in sheet and skip method to find column by name
</commit_message>
<xml_diff>
--- a/LandRegistryProject/TestDatas/TittleNumer.xlsx
+++ b/LandRegistryProject/TestDatas/TittleNumer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amos.Awaghade\source\repos\LandRegistryBulk-Discharge-Automation\LandRegistryProject\TestDatas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB85685A-E557-444A-8834-2B23660E7B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6333AA5-45F0-491B-811A-A21B03028194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{400498CB-F334-4E68-B062-A427E2481F8E}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1934" uniqueCount="1934">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1933" uniqueCount="1933">
   <si>
     <t>Daily Download</t>
   </si>
@@ -5458,397 +5458,394 @@
     <t>HP810130/Q946JHT/218</t>
   </si>
   <si>
+    <t>HD602384</t>
+  </si>
+  <si>
+    <t>1 Slater Way Ilkeston DE7 4SL</t>
+  </si>
+  <si>
+    <t>DY533669</t>
+  </si>
+  <si>
+    <t> 1 Slater Way, Ilkeston (DE7 4SL)</t>
+  </si>
+  <si>
+    <t>DY533669/W056JHT/218</t>
+  </si>
+  <si>
+    <t>54 Pius Avenue Lincoln LN6 9XT</t>
+  </si>
+  <si>
+    <t>LL393907</t>
+  </si>
+  <si>
+    <t>54 Pius Avenue, North Hykeham, Lincoln (LN6 9XT)</t>
+  </si>
+  <si>
+    <t> LL393907/S256JHT/218</t>
+  </si>
+  <si>
+    <t>2 Wilson Court Deepcut Camberley GU16 6FA</t>
+  </si>
+  <si>
+    <t>SY866329</t>
+  </si>
+  <si>
+    <t>2 Wilson Court, Deepcut, Camberley (GU16 6FA)</t>
+  </si>
+  <si>
+    <t>SY866329/X356JHT/218</t>
+  </si>
+  <si>
+    <t>28 Pintall close East Tilbury RM18 8FJ</t>
+  </si>
+  <si>
+    <t>EX969193</t>
+  </si>
+  <si>
+    <t>28 Pintail Close, East Tilbury, Tilbury (RM18 8FJ)</t>
+  </si>
+  <si>
+    <t>EX969193/Q656JHT/218</t>
+  </si>
+  <si>
+    <t>3 Pankhurst Close West Bromwich B70 0LW</t>
+  </si>
+  <si>
+    <t>MM128202</t>
+  </si>
+  <si>
+    <t>3 Pankhurst Close, West Bromwich And Parking Spaces (B70 0LW)</t>
+  </si>
+  <si>
+    <t>MM128202/L756JHT/218</t>
+  </si>
+  <si>
+    <t>41 Wincham Avenue Liverpool L24 1WS</t>
+  </si>
+  <si>
+    <t>MS687954</t>
+  </si>
+  <si>
+    <t>41 Wincham Avenue, Liverpool (L24 1WS)</t>
+  </si>
+  <si>
+    <t>MS687954/K856JHT/218</t>
+  </si>
+  <si>
+    <t>6, Northcote Avenue Lancashire OL1 4EH Oldham</t>
+  </si>
+  <si>
+    <t>MAN229892</t>
+  </si>
+  <si>
+    <t>6 Northcote Avenue, Oldham (OL1 4EH)</t>
+  </si>
+  <si>
+    <t> MAN229892/T856JHT/218</t>
+  </si>
+  <si>
+    <t>6 Woodland Crescent Halifax HX2 8WF</t>
+  </si>
+  <si>
+    <t>YY165413</t>
+  </si>
+  <si>
+    <t>6 Woodland Crescent, Halifax (HX2 8WF)</t>
+  </si>
+  <si>
+    <t>YY165413/Z956JHT/218</t>
+  </si>
+  <si>
+    <t>3 Sassoon Crescent Stowmarket IP14 1WA</t>
+  </si>
+  <si>
+    <t>SK382337</t>
+  </si>
+  <si>
+    <t> 3 Sassoon Crescent, Stowmarket (IP14 1WA)</t>
+  </si>
+  <si>
+    <t>SK382337/T066JHT/218</t>
+  </si>
+  <si>
+    <t>6 Teal Close Houghton Le Spring DH5 0GY Hetton Le Hole</t>
+  </si>
+  <si>
+    <t>TY534491</t>
+  </si>
+  <si>
+    <t> 6 Teal Close, Hetton-Le-Hole, Houghton Le Spring (DH5 0GY)</t>
+  </si>
+  <si>
+    <t>TY534491/V166JHT/218</t>
+  </si>
+  <si>
+    <t>11 Monastery Gardens Shepshed LE12 9FQ</t>
+  </si>
+  <si>
+    <t>LT482273</t>
+  </si>
+  <si>
+    <t>11 Monastery Gardens, Shepshed, Loughborough (LE12 9FQ)</t>
+  </si>
+  <si>
+    <t>LT482273/V266JHT/218</t>
+  </si>
+  <si>
+    <t>23 Hopkins Way York YO42 1AN</t>
+  </si>
+  <si>
+    <t>YEA90467</t>
+  </si>
+  <si>
+    <t>23 Hopkin Way, Pocklington, York (YO42 1AN)</t>
+  </si>
+  <si>
+    <t>YEA90467/M366JHT/218</t>
+  </si>
+  <si>
+    <t>7 Hundleby Court Cramlington NE23 1AS</t>
+  </si>
+  <si>
+    <t>ND195408</t>
+  </si>
+  <si>
+    <t>7 Hundleby Court, St. Nicholas Manor, Cramlington (NE23 1AS)</t>
+  </si>
+  <si>
+    <t>ND195408/J566JHT/218</t>
+  </si>
+  <si>
+    <t>22 Farmers Way Coalville LE67 2EG</t>
+  </si>
+  <si>
+    <t>LT510619</t>
+  </si>
+  <si>
+    <t> 22 Farmers Way, Hugglescote, Coalville (LE67 2EG)</t>
+  </si>
+  <si>
+    <t> LT510619/E666JHT/218</t>
+  </si>
+  <si>
+    <t>5 Harrier Way Norton Canes Cannock WS11 9AR</t>
+  </si>
+  <si>
+    <t>SF659628</t>
+  </si>
+  <si>
+    <t>5 Harrier Way, Norton Canes, Cannock (WS11 9AR)</t>
+  </si>
+  <si>
+    <t>SF659628/H676JHT/218</t>
+  </si>
+  <si>
+    <t>306 Hartsbourne Avenue Liverpool L25 2TD</t>
+  </si>
+  <si>
+    <t>MS672181</t>
+  </si>
+  <si>
+    <t>306 Hartsbourne Avenue, Liverpool (L25 2TD)</t>
+  </si>
+  <si>
+    <t> MS672181/F776JHT/218</t>
+  </si>
+  <si>
+    <t>77 1 Celmeres Court Springfield Road CM2 6JG Chelmsford</t>
+  </si>
+  <si>
+    <t>EX945892</t>
+  </si>
+  <si>
+    <t>1, Celmeres Court, 77 Springfield Road, Chelmsford (CM2 6JG)</t>
+  </si>
+  <si>
+    <t>EX945892/I786JHT/218</t>
+  </si>
+  <si>
+    <t>41 305 Glow Court Rookwod Way London E3 2XF</t>
+  </si>
+  <si>
+    <t>AGL509727</t>
+  </si>
+  <si>
+    <t> Flat 305, Glow Court, 41 Rookwood Way, London (E3 2XF)</t>
+  </si>
+  <si>
+    <t>AGL509727/H886JHT/218</t>
+  </si>
+  <si>
+    <t>23 Telford Road Winnington CW8 4YN</t>
+  </si>
+  <si>
+    <t>CH673009</t>
+  </si>
+  <si>
+    <t>23 Telford Road, Northwich (CW8 4YN)</t>
+  </si>
+  <si>
+    <t>CH673009/V886JHT/218</t>
+  </si>
+  <si>
+    <t>1 Stratford Way Bicester OX26 1BY</t>
+  </si>
+  <si>
+    <t>ON346247</t>
+  </si>
+  <si>
+    <t>1 Stratford Way, Bicester (OX26 1BY)</t>
+  </si>
+  <si>
+    <t>ON346247/J296JHT/218</t>
+  </si>
+  <si>
+    <t>9 West End Close Chippenham SN14 0FN</t>
+  </si>
+  <si>
+    <t>WT432310</t>
+  </si>
+  <si>
+    <t> 9 West End Close, Chippenham (SN14 0FN)</t>
+  </si>
+  <si>
+    <t>WT432310/E396JHT/218</t>
+  </si>
+  <si>
+    <t>20 Furnace Lane Swadlincote DE11 9QF</t>
+  </si>
+  <si>
+    <t>DY529578</t>
+  </si>
+  <si>
+    <t>20 Furnace Lane, Castle Gresley, Swadlincote (DE11 9QF)</t>
+  </si>
+  <si>
+    <t>DY529578/W396JHT/218</t>
+  </si>
+  <si>
+    <t>21 Stroothers Place Bradford Tyersal BD4 0BN</t>
+  </si>
+  <si>
+    <t>YY117941</t>
+  </si>
+  <si>
+    <t>21 Stroothers Place, Bradford (BD4 0BN)</t>
+  </si>
+  <si>
+    <t>YY117941/I596JHT/218</t>
+  </si>
+  <si>
+    <t>7 Flax Furrow Stratford Upon Avon CV37 0ED</t>
+  </si>
+  <si>
+    <t>WK493026</t>
+  </si>
+  <si>
+    <t>7 Flax Furrow, Stratford-Upon-Avon (CV37 0ED)</t>
+  </si>
+  <si>
+    <t>WK493026/P696JHT/218</t>
+  </si>
+  <si>
+    <t>23 Grange Road Huddersfield HD7 4QZ</t>
+  </si>
+  <si>
+    <t>YY110617/Y507JHT/218</t>
+  </si>
+  <si>
+    <t>25 Casson Gardens Thornaby TS17 0FU</t>
+  </si>
+  <si>
+    <t>CE241619</t>
+  </si>
+  <si>
+    <t>25 Casson Gardens, Thornaby, Stockton-On-Tees (TS17 0FU)</t>
+  </si>
+  <si>
+    <t>CE241619/P607JHT/218</t>
+  </si>
+  <si>
+    <t>52 Walker Road Northwich CW8 4UD</t>
+  </si>
+  <si>
+    <t>CH679826</t>
+  </si>
+  <si>
+    <t>52 Walker Road, Northwich (CW8 4UD)</t>
+  </si>
+  <si>
+    <t>CH679826/T617JHT/218</t>
+  </si>
+  <si>
+    <t>1 Staley Grove Bridgnorth WV16 6FB</t>
+  </si>
+  <si>
+    <t>SL257977</t>
+  </si>
+  <si>
+    <t>1 Staley Grove, Highley, Bridgnorth (WV16 6FB)</t>
+  </si>
+  <si>
+    <t>SL257977/T717JHT/218</t>
+  </si>
+  <si>
+    <t>15 Ivie Place Salisbury SP2 9GL</t>
+  </si>
+  <si>
+    <t>WT451944</t>
+  </si>
+  <si>
+    <t>15 Ivie Place, Salisbury (SP2 9GL)</t>
+  </si>
+  <si>
+    <t>WT451944/T817JHT/218</t>
+  </si>
+  <si>
+    <t>86 Hutchins Way Basingstoke RG24 9NG</t>
+  </si>
+  <si>
+    <t>HP831612</t>
+  </si>
+  <si>
+    <t>86 Hutchins Way, Basingstoke (RG24 9NG)</t>
+  </si>
+  <si>
+    <t>HP831612/J227JHT/218</t>
+  </si>
+  <si>
+    <t>17 Mary Way Clitheroe BB7 1FL</t>
+  </si>
+  <si>
+    <t>LAN223138</t>
+  </si>
+  <si>
+    <t>17 Mary Way, Clitheroe (BB7 1FL)</t>
+  </si>
+  <si>
+    <t>LAN223138/S427JHT/218</t>
+  </si>
+  <si>
+    <t>inbox</t>
+  </si>
+  <si>
+    <t>10 Caretakers Close Melksham SN12 8FR</t>
+  </si>
+  <si>
+    <t>WT464447</t>
+  </si>
+  <si>
+    <t>10 Caretakers Close, Melksham (SN12 8FR)</t>
+  </si>
+  <si>
+    <t>WT464447/R527JHT/218</t>
+  </si>
+  <si>
     <t>31 Wallace Green Way, Walkern, Stevenage (SG2 7FB)</t>
   </si>
   <si>
-    <t>HD602384</t>
-  </si>
-  <si>
-    <t>1 Slater Way Ilkeston DE7 4SL</t>
-  </si>
-  <si>
-    <t>DY533669</t>
-  </si>
-  <si>
-    <t> 1 Slater Way, Ilkeston (DE7 4SL)</t>
-  </si>
-  <si>
-    <t>DY533669/W056JHT/218</t>
-  </si>
-  <si>
-    <t>54 Pius Avenue Lincoln LN6 9XT</t>
-  </si>
-  <si>
-    <t>LL393907</t>
-  </si>
-  <si>
-    <t>54 Pius Avenue, North Hykeham, Lincoln (LN6 9XT)</t>
-  </si>
-  <si>
-    <t> LL393907/S256JHT/218</t>
-  </si>
-  <si>
-    <t>2 Wilson Court Deepcut Camberley GU16 6FA</t>
-  </si>
-  <si>
-    <t>SY866329</t>
-  </si>
-  <si>
-    <t>2 Wilson Court, Deepcut, Camberley (GU16 6FA)</t>
-  </si>
-  <si>
-    <t>SY866329/X356JHT/218</t>
-  </si>
-  <si>
-    <t>28 Pintall close East Tilbury RM18 8FJ</t>
-  </si>
-  <si>
-    <t>EX969193</t>
-  </si>
-  <si>
-    <t>28 Pintail Close, East Tilbury, Tilbury (RM18 8FJ)</t>
-  </si>
-  <si>
-    <t>EX969193/Q656JHT/218</t>
-  </si>
-  <si>
-    <t>3 Pankhurst Close West Bromwich B70 0LW</t>
-  </si>
-  <si>
-    <t>MM128202</t>
-  </si>
-  <si>
-    <t>3 Pankhurst Close, West Bromwich And Parking Spaces (B70 0LW)</t>
-  </si>
-  <si>
-    <t>MM128202/L756JHT/218</t>
-  </si>
-  <si>
-    <t>41 Wincham Avenue Liverpool L24 1WS</t>
-  </si>
-  <si>
-    <t>MS687954</t>
-  </si>
-  <si>
-    <t>41 Wincham Avenue, Liverpool (L24 1WS)</t>
-  </si>
-  <si>
-    <t>MS687954/K856JHT/218</t>
-  </si>
-  <si>
-    <t>6, Northcote Avenue Lancashire OL1 4EH Oldham</t>
-  </si>
-  <si>
-    <t>MAN229892</t>
-  </si>
-  <si>
-    <t>6 Northcote Avenue, Oldham (OL1 4EH)</t>
-  </si>
-  <si>
-    <t> MAN229892/T856JHT/218</t>
-  </si>
-  <si>
-    <t>6 Woodland Crescent Halifax HX2 8WF</t>
-  </si>
-  <si>
-    <t>YY165413</t>
-  </si>
-  <si>
-    <t>6 Woodland Crescent, Halifax (HX2 8WF)</t>
-  </si>
-  <si>
-    <t>YY165413/Z956JHT/218</t>
-  </si>
-  <si>
-    <t>3 Sassoon Crescent Stowmarket IP14 1WA</t>
-  </si>
-  <si>
-    <t>SK382337</t>
-  </si>
-  <si>
-    <t> 3 Sassoon Crescent, Stowmarket (IP14 1WA)</t>
-  </si>
-  <si>
-    <t>SK382337/T066JHT/218</t>
-  </si>
-  <si>
-    <t>6 Teal Close Houghton Le Spring DH5 0GY Hetton Le Hole</t>
-  </si>
-  <si>
-    <t>TY534491</t>
-  </si>
-  <si>
-    <t> 6 Teal Close, Hetton-Le-Hole, Houghton Le Spring (DH5 0GY)</t>
-  </si>
-  <si>
-    <t>TY534491/V166JHT/218</t>
-  </si>
-  <si>
-    <t>11 Monastery Gardens Shepshed LE12 9FQ</t>
-  </si>
-  <si>
-    <t>LT482273</t>
-  </si>
-  <si>
-    <t>11 Monastery Gardens, Shepshed, Loughborough (LE12 9FQ)</t>
-  </si>
-  <si>
-    <t>LT482273/V266JHT/218</t>
-  </si>
-  <si>
-    <t>23 Hopkins Way York YO42 1AN</t>
-  </si>
-  <si>
-    <t>YEA90467</t>
-  </si>
-  <si>
-    <t>23 Hopkin Way, Pocklington, York (YO42 1AN)</t>
-  </si>
-  <si>
-    <t>YEA90467/M366JHT/218</t>
-  </si>
-  <si>
-    <t>7 Hundleby Court Cramlington NE23 1AS</t>
-  </si>
-  <si>
-    <t>ND195408</t>
-  </si>
-  <si>
-    <t>7 Hundleby Court, St. Nicholas Manor, Cramlington (NE23 1AS)</t>
-  </si>
-  <si>
-    <t>ND195408/J566JHT/218</t>
-  </si>
-  <si>
-    <t>22 Farmers Way Coalville LE67 2EG</t>
-  </si>
-  <si>
-    <t>LT510619</t>
-  </si>
-  <si>
-    <t> 22 Farmers Way, Hugglescote, Coalville (LE67 2EG)</t>
-  </si>
-  <si>
-    <t> LT510619/E666JHT/218</t>
-  </si>
-  <si>
-    <t>5 Harrier Way Norton Canes Cannock WS11 9AR</t>
-  </si>
-  <si>
-    <t>SF659628</t>
-  </si>
-  <si>
-    <t>5 Harrier Way, Norton Canes, Cannock (WS11 9AR)</t>
-  </si>
-  <si>
-    <t>SF659628/H676JHT/218</t>
-  </si>
-  <si>
-    <t>306 Hartsbourne Avenue Liverpool L25 2TD</t>
-  </si>
-  <si>
-    <t>MS672181</t>
-  </si>
-  <si>
-    <t>306 Hartsbourne Avenue, Liverpool (L25 2TD)</t>
-  </si>
-  <si>
-    <t> MS672181/F776JHT/218</t>
-  </si>
-  <si>
-    <t>77 1 Celmeres Court Springfield Road CM2 6JG Chelmsford</t>
-  </si>
-  <si>
-    <t>EX945892</t>
-  </si>
-  <si>
-    <t>1, Celmeres Court, 77 Springfield Road, Chelmsford (CM2 6JG)</t>
-  </si>
-  <si>
-    <t>EX945892/I786JHT/218</t>
-  </si>
-  <si>
-    <t>41 305 Glow Court Rookwod Way London E3 2XF</t>
-  </si>
-  <si>
-    <t>AGL509727</t>
-  </si>
-  <si>
-    <t> Flat 305, Glow Court, 41 Rookwood Way, London (E3 2XF)</t>
-  </si>
-  <si>
-    <t>AGL509727/H886JHT/218</t>
-  </si>
-  <si>
-    <t>23 Telford Road Winnington CW8 4YN</t>
-  </si>
-  <si>
-    <t>CH673009</t>
-  </si>
-  <si>
-    <t>23 Telford Road, Northwich (CW8 4YN)</t>
-  </si>
-  <si>
-    <t>CH673009/V886JHT/218</t>
-  </si>
-  <si>
-    <t>1 Stratford Way Bicester OX26 1BY</t>
-  </si>
-  <si>
-    <t>ON346247</t>
-  </si>
-  <si>
-    <t>1 Stratford Way, Bicester (OX26 1BY)</t>
-  </si>
-  <si>
-    <t>ON346247/J296JHT/218</t>
-  </si>
-  <si>
-    <t>9 West End Close Chippenham SN14 0FN</t>
-  </si>
-  <si>
-    <t>WT432310</t>
-  </si>
-  <si>
-    <t> 9 West End Close, Chippenham (SN14 0FN)</t>
-  </si>
-  <si>
-    <t>WT432310/E396JHT/218</t>
-  </si>
-  <si>
-    <t>20 Furnace Lane Swadlincote DE11 9QF</t>
-  </si>
-  <si>
-    <t>DY529578</t>
-  </si>
-  <si>
-    <t>20 Furnace Lane, Castle Gresley, Swadlincote (DE11 9QF)</t>
-  </si>
-  <si>
-    <t>DY529578/W396JHT/218</t>
-  </si>
-  <si>
-    <t>21 Stroothers Place Bradford Tyersal BD4 0BN</t>
-  </si>
-  <si>
-    <t>YY117941</t>
-  </si>
-  <si>
-    <t>21 Stroothers Place, Bradford (BD4 0BN)</t>
-  </si>
-  <si>
-    <t>YY117941/I596JHT/218</t>
-  </si>
-  <si>
-    <t>7 Flax Furrow Stratford Upon Avon CV37 0ED</t>
-  </si>
-  <si>
-    <t>WK493026</t>
-  </si>
-  <si>
-    <t>7 Flax Furrow, Stratford-Upon-Avon (CV37 0ED)</t>
-  </si>
-  <si>
-    <t>WK493026/P696JHT/218</t>
-  </si>
-  <si>
-    <t>23 Grange Road Huddersfield HD7 4QZ</t>
-  </si>
-  <si>
-    <t>YY110617/Y507JHT/218</t>
-  </si>
-  <si>
-    <t>25 Casson Gardens Thornaby TS17 0FU</t>
-  </si>
-  <si>
-    <t>CE241619</t>
-  </si>
-  <si>
-    <t>25 Casson Gardens, Thornaby, Stockton-On-Tees (TS17 0FU)</t>
-  </si>
-  <si>
-    <t>CE241619/P607JHT/218</t>
-  </si>
-  <si>
-    <t>52 Walker Road Northwich CW8 4UD</t>
-  </si>
-  <si>
-    <t>CH679826</t>
-  </si>
-  <si>
-    <t>52 Walker Road, Northwich (CW8 4UD)</t>
-  </si>
-  <si>
-    <t>CH679826/T617JHT/218</t>
-  </si>
-  <si>
-    <t>1 Staley Grove Bridgnorth WV16 6FB</t>
-  </si>
-  <si>
-    <t>SL257977</t>
-  </si>
-  <si>
-    <t>1 Staley Grove, Highley, Bridgnorth (WV16 6FB)</t>
-  </si>
-  <si>
-    <t>SL257977/T717JHT/218</t>
-  </si>
-  <si>
-    <t>15 Ivie Place Salisbury SP2 9GL</t>
-  </si>
-  <si>
-    <t>WT451944</t>
-  </si>
-  <si>
-    <t>15 Ivie Place, Salisbury (SP2 9GL)</t>
-  </si>
-  <si>
-    <t>WT451944/T817JHT/218</t>
-  </si>
-  <si>
-    <t>86 Hutchins Way Basingstoke RG24 9NG</t>
-  </si>
-  <si>
-    <t>HP831612</t>
-  </si>
-  <si>
-    <t>86 Hutchins Way, Basingstoke (RG24 9NG)</t>
-  </si>
-  <si>
-    <t>HP831612/J227JHT/218</t>
-  </si>
-  <si>
-    <t>17 Mary Way Clitheroe BB7 1FL</t>
-  </si>
-  <si>
-    <t>LAN223138</t>
-  </si>
-  <si>
-    <t>17 Mary Way, Clitheroe (BB7 1FL)</t>
-  </si>
-  <si>
-    <t>LAN223138/S427JHT/218</t>
-  </si>
-  <si>
-    <t>inbox</t>
-  </si>
-  <si>
-    <t>10 Caretakers Close Melksham SN12 8FR</t>
-  </si>
-  <si>
-    <t>WT464447</t>
-  </si>
-  <si>
-    <t>10 Caretakers Close, Melksham (SN12 8FR)</t>
-  </si>
-  <si>
-    <t>WT464447/R527JHT/218</t>
-  </si>
-  <si>
-    <t>HD602384/T977JHT/218</t>
-  </si>
-  <si>
-    <t>HD602384/V977JHT/218</t>
+    <t>HD602384/L099LHT/221</t>
   </si>
 </sst>
 </file>
@@ -6375,36 +6372,6 @@
   <dxfs count="42">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -6765,6 +6732,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="ff9c0006"/>
       </font>
       <fill>
@@ -6818,8 +6815,8 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>3036</xdr:row>
-      <xdr:rowOff>35223</xdr:rowOff>
+      <xdr:row>3037</xdr:row>
+      <xdr:rowOff>35221</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6836,8 +6833,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="10706302" y="1570768"/>
-          <a:ext cx="309738" cy="577891097"/>
+          <a:off x="8817951" y="1571729"/>
+          <a:ext cx="308680" cy="578300670"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6915,9 +6912,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>3035</xdr:row>
-      <xdr:rowOff>160604</xdr:rowOff>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>3036</xdr:row>
+      <xdr:rowOff>160602</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7307,15 +7304,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8018EBFC-BBDD-47D5-8A8F-DFE2D059D3E8}">
-  <dimension ref="A1:R488"/>
+  <dimension ref="A1:R489"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B442" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection activeCell="A49" sqref="A49"/>
-      <selection pane="topRight" activeCell="M488" sqref="M488"/>
+    <sheetView tabSelected="1" topLeftCell="A450" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K488" sqref="K488"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="9.140625" customWidth="1" style="22"/>
     <col min="3" max="3" width="13.42578125" customWidth="1" style="24"/>
@@ -7333,7 +7328,8 @@
     <col min="15" max="15" width="14.42578125" customWidth="1" style="24"/>
     <col min="16" max="16" width="9.140625" customWidth="1" style="22"/>
     <col min="17" max="17" width="59" customWidth="1" style="22"/>
-    <col min="18" max="16384" width="9.140625" customWidth="1" style="22"/>
+    <col min="18" max="24" width="9.140625" customWidth="1" style="22"/>
+    <col min="25" max="16384" width="9.140625" customWidth="1" style="22"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1" s="6" customFormat="1">
@@ -29266,27 +29262,11 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="455">
-      <c r="A455" s="22">
-        <v>3</v>
-      </c>
-      <c r="D455" s="22" t="s">
+    <row r="455" ht="15.75">
+      <c r="C455" s="28"/>
+      <c r="G455" s="24"/>
+      <c r="I455" s="23" t="s">
         <v>1803</v>
-      </c>
-      <c r="E455" s="22">
-        <v>55555</v>
-      </c>
-      <c r="I455" s="23" t="s">
-        <v>1804</v>
-      </c>
-      <c r="J455" s="21" t="s">
-        <v>1803</v>
-      </c>
-      <c r="K455" s="22" t="s">
-        <v>1932</v>
-      </c>
-      <c r="M455" s="22" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="456" ht="15" customHeight="1">
@@ -29297,7 +29277,7 @@
         <v>45334</v>
       </c>
       <c r="D456" s="22" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="E456" s="21">
         <v>869953</v>
@@ -29312,13 +29292,13 @@
         <v>31</v>
       </c>
       <c r="I456" s="23" t="s">
+        <v>1805</v>
+      </c>
+      <c r="J456" s="68" t="s">
         <v>1806</v>
       </c>
-      <c r="J456" s="68" t="s">
+      <c r="K456" s="22" t="s">
         <v>1807</v>
-      </c>
-      <c r="K456" s="22" t="s">
-        <v>1808</v>
       </c>
       <c r="L456" s="22" t="s">
         <v>866</v>
@@ -29344,7 +29324,7 @@
         <v>45334</v>
       </c>
       <c r="D457" s="22" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="E457" s="21">
         <v>881387</v>
@@ -29359,13 +29339,13 @@
         <v>31</v>
       </c>
       <c r="I457" s="23" t="s">
+        <v>1809</v>
+      </c>
+      <c r="J457" s="68" t="s">
         <v>1810</v>
       </c>
-      <c r="J457" s="68" t="s">
+      <c r="K457" s="68" t="s">
         <v>1811</v>
-      </c>
-      <c r="K457" s="68" t="s">
-        <v>1812</v>
       </c>
       <c r="L457" s="22" t="s">
         <v>866</v>
@@ -29391,7 +29371,7 @@
         <v>45334</v>
       </c>
       <c r="D458" s="22" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
       <c r="E458" s="21">
         <v>917109</v>
@@ -29406,13 +29386,13 @@
         <v>31</v>
       </c>
       <c r="I458" s="23" t="s">
+        <v>1813</v>
+      </c>
+      <c r="J458" s="68" t="s">
         <v>1814</v>
       </c>
-      <c r="J458" s="68" t="s">
+      <c r="K458" s="68" t="s">
         <v>1815</v>
-      </c>
-      <c r="K458" s="68" t="s">
-        <v>1816</v>
       </c>
       <c r="L458" s="22" t="s">
         <v>866</v>
@@ -29438,7 +29418,7 @@
         <v>45334</v>
       </c>
       <c r="D459" s="22" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="E459" s="21">
         <v>803129</v>
@@ -29453,13 +29433,13 @@
         <v>31</v>
       </c>
       <c r="I459" s="23" t="s">
+        <v>1817</v>
+      </c>
+      <c r="J459" s="68" t="s">
         <v>1818</v>
       </c>
-      <c r="J459" s="68" t="s">
+      <c r="K459" s="68" t="s">
         <v>1819</v>
-      </c>
-      <c r="K459" s="68" t="s">
-        <v>1820</v>
       </c>
       <c r="L459" s="22" t="s">
         <v>866</v>
@@ -29485,7 +29465,7 @@
         <v>45334</v>
       </c>
       <c r="D460" s="22" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="E460" s="21">
         <v>865333</v>
@@ -29500,13 +29480,13 @@
         <v>31</v>
       </c>
       <c r="I460" s="23" t="s">
+        <v>1821</v>
+      </c>
+      <c r="J460" s="68" t="s">
         <v>1822</v>
       </c>
-      <c r="J460" s="68" t="s">
+      <c r="K460" s="68" t="s">
         <v>1823</v>
-      </c>
-      <c r="K460" s="68" t="s">
-        <v>1824</v>
       </c>
       <c r="L460" s="22" t="s">
         <v>866</v>
@@ -29532,7 +29512,7 @@
         <v>45334</v>
       </c>
       <c r="D461" s="22" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="E461" s="21">
         <v>990861</v>
@@ -29547,13 +29527,13 @@
         <v>31</v>
       </c>
       <c r="I461" s="23" t="s">
+        <v>1825</v>
+      </c>
+      <c r="J461" s="68" t="s">
         <v>1826</v>
       </c>
-      <c r="J461" s="68" t="s">
+      <c r="K461" s="68" t="s">
         <v>1827</v>
-      </c>
-      <c r="K461" s="68" t="s">
-        <v>1828</v>
       </c>
       <c r="L461" s="22" t="s">
         <v>866</v>
@@ -29579,7 +29559,7 @@
         <v>45334</v>
       </c>
       <c r="D462" s="22" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="E462" s="21">
         <v>618051</v>
@@ -29594,13 +29574,13 @@
         <v>31</v>
       </c>
       <c r="I462" s="23" t="s">
+        <v>1829</v>
+      </c>
+      <c r="J462" s="68" t="s">
         <v>1830</v>
       </c>
-      <c r="J462" s="68" t="s">
+      <c r="K462" s="68" t="s">
         <v>1831</v>
-      </c>
-      <c r="K462" s="68" t="s">
-        <v>1832</v>
       </c>
       <c r="L462" s="22" t="s">
         <v>866</v>
@@ -29626,7 +29606,7 @@
         <v>45334</v>
       </c>
       <c r="D463" s="22" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="E463" s="21">
         <v>968744</v>
@@ -29641,13 +29621,13 @@
         <v>31</v>
       </c>
       <c r="I463" s="23" t="s">
+        <v>1833</v>
+      </c>
+      <c r="J463" s="68" t="s">
         <v>1834</v>
       </c>
-      <c r="J463" s="68" t="s">
+      <c r="K463" s="68" t="s">
         <v>1835</v>
-      </c>
-      <c r="K463" s="68" t="s">
-        <v>1836</v>
       </c>
       <c r="L463" s="22" t="s">
         <v>866</v>
@@ -29673,7 +29653,7 @@
         <v>45334</v>
       </c>
       <c r="D464" s="22" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="E464" s="21">
         <v>791508</v>
@@ -29688,13 +29668,13 @@
         <v>31</v>
       </c>
       <c r="I464" s="23" t="s">
+        <v>1837</v>
+      </c>
+      <c r="J464" s="68" t="s">
         <v>1838</v>
       </c>
-      <c r="J464" s="68" t="s">
+      <c r="K464" s="68" t="s">
         <v>1839</v>
-      </c>
-      <c r="K464" s="68" t="s">
-        <v>1840</v>
       </c>
       <c r="L464" s="22" t="s">
         <v>866</v>
@@ -29720,7 +29700,7 @@
         <v>45334</v>
       </c>
       <c r="D465" s="22" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
       <c r="E465" s="21">
         <v>682738</v>
@@ -29735,13 +29715,13 @@
         <v>31</v>
       </c>
       <c r="I465" s="23" t="s">
+        <v>1841</v>
+      </c>
+      <c r="J465" s="68" t="s">
         <v>1842</v>
       </c>
-      <c r="J465" s="68" t="s">
+      <c r="K465" s="68" t="s">
         <v>1843</v>
-      </c>
-      <c r="K465" s="68" t="s">
-        <v>1844</v>
       </c>
       <c r="L465" s="22" t="s">
         <v>866</v>
@@ -29767,7 +29747,7 @@
         <v>45334</v>
       </c>
       <c r="D466" s="22" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="E466" s="21">
         <v>696891</v>
@@ -29782,13 +29762,13 @@
         <v>31</v>
       </c>
       <c r="I466" s="23" t="s">
+        <v>1845</v>
+      </c>
+      <c r="J466" s="68" t="s">
         <v>1846</v>
       </c>
-      <c r="J466" s="68" t="s">
+      <c r="K466" s="68" t="s">
         <v>1847</v>
-      </c>
-      <c r="K466" s="68" t="s">
-        <v>1848</v>
       </c>
       <c r="L466" s="22" t="s">
         <v>866</v>
@@ -29814,7 +29794,7 @@
         <v>45334</v>
       </c>
       <c r="D467" s="22" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="E467" s="21">
         <v>866515</v>
@@ -29829,13 +29809,13 @@
         <v>31</v>
       </c>
       <c r="I467" s="23" t="s">
+        <v>1849</v>
+      </c>
+      <c r="J467" s="68" t="s">
         <v>1850</v>
       </c>
-      <c r="J467" s="68" t="s">
+      <c r="K467" s="68" t="s">
         <v>1851</v>
-      </c>
-      <c r="K467" s="68" t="s">
-        <v>1852</v>
       </c>
       <c r="L467" s="22" t="s">
         <v>866</v>
@@ -29861,7 +29841,7 @@
         <v>45334</v>
       </c>
       <c r="D468" s="22" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="E468" s="21">
         <v>822731</v>
@@ -29876,13 +29856,13 @@
         <v>31</v>
       </c>
       <c r="I468" s="23" t="s">
+        <v>1853</v>
+      </c>
+      <c r="J468" s="68" t="s">
         <v>1854</v>
       </c>
-      <c r="J468" s="68" t="s">
+      <c r="K468" s="68" t="s">
         <v>1855</v>
-      </c>
-      <c r="K468" s="68" t="s">
-        <v>1856</v>
       </c>
       <c r="L468" s="22" t="s">
         <v>866</v>
@@ -29908,7 +29888,7 @@
         <v>45334</v>
       </c>
       <c r="D469" s="22" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="E469" s="21">
         <v>860463</v>
@@ -29923,13 +29903,13 @@
         <v>31</v>
       </c>
       <c r="I469" s="72" t="s">
+        <v>1857</v>
+      </c>
+      <c r="J469" s="68" t="s">
         <v>1858</v>
       </c>
-      <c r="J469" s="68" t="s">
+      <c r="K469" s="68" t="s">
         <v>1859</v>
-      </c>
-      <c r="K469" s="68" t="s">
-        <v>1860</v>
       </c>
       <c r="L469" s="22" t="s">
         <v>866</v>
@@ -29955,7 +29935,7 @@
         <v>45334</v>
       </c>
       <c r="D470" s="22" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="E470" s="21">
         <v>942874</v>
@@ -29970,13 +29950,13 @@
         <v>31</v>
       </c>
       <c r="I470" s="72" t="s">
+        <v>1861</v>
+      </c>
+      <c r="J470" s="68" t="s">
         <v>1862</v>
       </c>
-      <c r="J470" s="68" t="s">
+      <c r="K470" s="68" t="s">
         <v>1863</v>
-      </c>
-      <c r="K470" s="68" t="s">
-        <v>1864</v>
       </c>
       <c r="L470" s="22" t="s">
         <v>866</v>
@@ -30002,7 +29982,7 @@
         <v>45334</v>
       </c>
       <c r="D471" s="22" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
       <c r="E471" s="21">
         <v>885630</v>
@@ -30017,13 +29997,13 @@
         <v>31</v>
       </c>
       <c r="I471" s="72" t="s">
+        <v>1865</v>
+      </c>
+      <c r="J471" s="68" t="s">
         <v>1866</v>
       </c>
-      <c r="J471" s="68" t="s">
+      <c r="K471" s="68" t="s">
         <v>1867</v>
-      </c>
-      <c r="K471" s="68" t="s">
-        <v>1868</v>
       </c>
       <c r="L471" s="22" t="s">
         <v>866</v>
@@ -30049,7 +30029,7 @@
         <v>45334</v>
       </c>
       <c r="D472" s="22" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="E472" s="21">
         <v>720363</v>
@@ -30064,13 +30044,13 @@
         <v>31</v>
       </c>
       <c r="I472" s="23" t="s">
+        <v>1869</v>
+      </c>
+      <c r="J472" s="68" t="s">
         <v>1870</v>
       </c>
-      <c r="J472" s="68" t="s">
+      <c r="K472" s="68" t="s">
         <v>1871</v>
-      </c>
-      <c r="K472" s="68" t="s">
-        <v>1872</v>
       </c>
       <c r="L472" s="22" t="s">
         <v>866</v>
@@ -30096,7 +30076,7 @@
         <v>45334</v>
       </c>
       <c r="D473" s="22" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="E473" s="21">
         <v>951008</v>
@@ -30111,13 +30091,13 @@
         <v>31</v>
       </c>
       <c r="I473" s="23" t="s">
+        <v>1873</v>
+      </c>
+      <c r="J473" s="68" t="s">
         <v>1874</v>
       </c>
-      <c r="J473" s="68" t="s">
+      <c r="K473" s="68" t="s">
         <v>1875</v>
-      </c>
-      <c r="K473" s="68" t="s">
-        <v>1876</v>
       </c>
       <c r="L473" s="22" t="s">
         <v>866</v>
@@ -30143,7 +30123,7 @@
         <v>45334</v>
       </c>
       <c r="D474" s="22" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="E474" s="21">
         <v>837884</v>
@@ -30158,13 +30138,13 @@
         <v>31</v>
       </c>
       <c r="I474" s="23" t="s">
+        <v>1877</v>
+      </c>
+      <c r="J474" s="68" t="s">
         <v>1878</v>
       </c>
-      <c r="J474" s="68" t="s">
+      <c r="K474" s="68" t="s">
         <v>1879</v>
-      </c>
-      <c r="K474" s="68" t="s">
-        <v>1880</v>
       </c>
       <c r="L474" s="22" t="s">
         <v>866</v>
@@ -30190,7 +30170,7 @@
         <v>45334</v>
       </c>
       <c r="D475" s="22" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="E475" s="21">
         <v>849393</v>
@@ -30205,13 +30185,13 @@
         <v>31</v>
       </c>
       <c r="I475" s="23" t="s">
+        <v>1881</v>
+      </c>
+      <c r="J475" s="68" t="s">
         <v>1882</v>
       </c>
-      <c r="J475" s="68" t="s">
+      <c r="K475" s="68" t="s">
         <v>1883</v>
-      </c>
-      <c r="K475" s="68" t="s">
-        <v>1884</v>
       </c>
       <c r="L475" s="22" t="s">
         <v>866</v>
@@ -30237,7 +30217,7 @@
         <v>45334</v>
       </c>
       <c r="D476" s="22" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="E476" s="21">
         <v>747206</v>
@@ -30252,13 +30232,13 @@
         <v>31</v>
       </c>
       <c r="I476" s="23" t="s">
+        <v>1885</v>
+      </c>
+      <c r="J476" s="68" t="s">
         <v>1886</v>
       </c>
-      <c r="J476" s="68" t="s">
+      <c r="K476" s="68" t="s">
         <v>1887</v>
-      </c>
-      <c r="K476" s="68" t="s">
-        <v>1888</v>
       </c>
       <c r="L476" s="22" t="s">
         <v>866</v>
@@ -30284,7 +30264,7 @@
         <v>45334</v>
       </c>
       <c r="D477" s="22" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="E477" s="21">
         <v>852917</v>
@@ -30299,13 +30279,13 @@
         <v>31</v>
       </c>
       <c r="I477" s="23" t="s">
+        <v>1889</v>
+      </c>
+      <c r="J477" s="68" t="s">
         <v>1890</v>
       </c>
-      <c r="J477" s="68" t="s">
+      <c r="K477" s="68" t="s">
         <v>1891</v>
-      </c>
-      <c r="K477" s="68" t="s">
-        <v>1892</v>
       </c>
       <c r="L477" s="22" t="s">
         <v>866</v>
@@ -30331,7 +30311,7 @@
         <v>45334</v>
       </c>
       <c r="D478" s="22" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="E478" s="21">
         <v>826182</v>
@@ -30346,13 +30326,13 @@
         <v>31</v>
       </c>
       <c r="I478" s="23" t="s">
+        <v>1893</v>
+      </c>
+      <c r="J478" s="68" t="s">
         <v>1894</v>
       </c>
-      <c r="J478" s="68" t="s">
+      <c r="K478" s="68" t="s">
         <v>1895</v>
-      </c>
-      <c r="K478" s="68" t="s">
-        <v>1896</v>
       </c>
       <c r="L478" s="22" t="s">
         <v>866</v>
@@ -30378,7 +30358,7 @@
         <v>45334</v>
       </c>
       <c r="D479" s="22" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="E479" s="21">
         <v>778098</v>
@@ -30393,13 +30373,13 @@
         <v>31</v>
       </c>
       <c r="I479" s="23" t="s">
+        <v>1897</v>
+      </c>
+      <c r="J479" s="68" t="s">
         <v>1898</v>
       </c>
-      <c r="J479" s="68" t="s">
+      <c r="K479" s="68" t="s">
         <v>1899</v>
-      </c>
-      <c r="K479" s="68" t="s">
-        <v>1900</v>
       </c>
       <c r="L479" s="22" t="s">
         <v>866</v>
@@ -30425,7 +30405,7 @@
         <v>45334</v>
       </c>
       <c r="D480" s="22" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="E480" s="21">
         <v>832644</v>
@@ -30446,7 +30426,7 @@
         <v>831</v>
       </c>
       <c r="K480" s="68" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
       <c r="L480" s="22" t="s">
         <v>866</v>
@@ -30472,7 +30452,7 @@
         <v>45334</v>
       </c>
       <c r="D481" s="22" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
       <c r="E481" s="21">
         <v>880275</v>
@@ -30487,13 +30467,13 @@
         <v>31</v>
       </c>
       <c r="I481" s="23" t="s">
+        <v>1903</v>
+      </c>
+      <c r="J481" s="68" t="s">
         <v>1904</v>
       </c>
-      <c r="J481" s="68" t="s">
+      <c r="K481" s="68" t="s">
         <v>1905</v>
-      </c>
-      <c r="K481" s="68" t="s">
-        <v>1906</v>
       </c>
       <c r="L481" s="22" t="s">
         <v>866</v>
@@ -30519,7 +30499,7 @@
         <v>45334</v>
       </c>
       <c r="D482" s="22" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="E482" s="21">
         <v>840914</v>
@@ -30534,13 +30514,13 @@
         <v>31</v>
       </c>
       <c r="I482" s="23" t="s">
+        <v>1907</v>
+      </c>
+      <c r="J482" s="68" t="s">
         <v>1908</v>
       </c>
-      <c r="J482" s="68" t="s">
+      <c r="K482" s="68" t="s">
         <v>1909</v>
-      </c>
-      <c r="K482" s="68" t="s">
-        <v>1910</v>
       </c>
       <c r="L482" s="22" t="s">
         <v>866</v>
@@ -30566,7 +30546,7 @@
         <v>45334</v>
       </c>
       <c r="D483" s="22" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="E483" s="21">
         <v>872163</v>
@@ -30581,13 +30561,13 @@
         <v>31</v>
       </c>
       <c r="I483" s="23" t="s">
+        <v>1911</v>
+      </c>
+      <c r="J483" s="68" t="s">
         <v>1912</v>
       </c>
-      <c r="J483" s="68" t="s">
+      <c r="K483" s="68" t="s">
         <v>1913</v>
-      </c>
-      <c r="K483" s="68" t="s">
-        <v>1914</v>
       </c>
       <c r="L483" s="22" t="s">
         <v>866</v>
@@ -30613,7 +30593,7 @@
         <v>45334</v>
       </c>
       <c r="D484" s="22" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="E484" s="21">
         <v>943025</v>
@@ -30628,13 +30608,13 @@
         <v>31</v>
       </c>
       <c r="I484" s="23" t="s">
+        <v>1915</v>
+      </c>
+      <c r="J484" s="68" t="s">
         <v>1916</v>
       </c>
-      <c r="J484" s="68" t="s">
+      <c r="K484" s="68" t="s">
         <v>1917</v>
-      </c>
-      <c r="K484" s="68" t="s">
-        <v>1918</v>
       </c>
       <c r="L484" s="22" t="s">
         <v>866</v>
@@ -30660,7 +30640,7 @@
         <v>45334</v>
       </c>
       <c r="D485" s="22" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="E485" s="21">
         <v>870491</v>
@@ -30675,13 +30655,13 @@
         <v>31</v>
       </c>
       <c r="I485" s="23" t="s">
+        <v>1919</v>
+      </c>
+      <c r="J485" s="68" t="s">
         <v>1920</v>
       </c>
-      <c r="J485" s="68" t="s">
+      <c r="K485" s="68" t="s">
         <v>1921</v>
-      </c>
-      <c r="K485" s="68" t="s">
-        <v>1922</v>
       </c>
       <c r="L485" s="22" t="s">
         <v>866</v>
@@ -30707,7 +30687,7 @@
         <v>45334</v>
       </c>
       <c r="D486" s="22" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
       <c r="E486" s="21">
         <v>888839</v>
@@ -30722,13 +30702,13 @@
         <v>31</v>
       </c>
       <c r="I486" s="23" t="s">
+        <v>1923</v>
+      </c>
+      <c r="J486" s="68" t="s">
         <v>1924</v>
       </c>
-      <c r="J486" s="68" t="s">
+      <c r="K486" s="68" t="s">
         <v>1925</v>
-      </c>
-      <c r="K486" s="68" t="s">
-        <v>1926</v>
       </c>
       <c r="L486" s="22" t="s">
         <v>866</v>
@@ -30748,13 +30728,13 @@
     </row>
     <row r="487" ht="15" customHeight="1">
       <c r="B487" s="22" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="C487" s="24">
         <v>45334</v>
       </c>
       <c r="D487" s="22" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="E487" s="22">
         <v>743506</v>
@@ -30769,13 +30749,13 @@
         <v>31</v>
       </c>
       <c r="I487" s="23" t="s">
+        <v>1928</v>
+      </c>
+      <c r="J487" s="68" t="s">
         <v>1929</v>
       </c>
-      <c r="J487" s="68" t="s">
+      <c r="K487" s="68" t="s">
         <v>1930</v>
-      </c>
-      <c r="K487" s="68" t="s">
-        <v>1931</v>
       </c>
       <c r="L487" s="22" t="s">
         <v>866</v>
@@ -30784,26 +30764,67 @@
         <v>147</v>
       </c>
     </row>
-    <row r="488">
+    <row r="488" ht="31.5">
       <c r="A488" s="22">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="B488" s="22" t="s">
+        <v>1926</v>
+      </c>
+      <c r="C488" s="24">
+        <v>45334</v>
       </c>
       <c r="D488" s="22" t="s">
+        <v>1931</v>
+      </c>
+      <c r="E488" s="22">
+        <v>743506</v>
+      </c>
+      <c r="F488" s="22" t="s">
+        <v>350</v>
+      </c>
+      <c r="G488" s="24">
+        <v>45335</v>
+      </c>
+      <c r="H488" s="25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="489" ht="31.5">
+      <c r="A489" s="22">
+        <v>1</v>
+      </c>
+      <c r="B489" s="22" t="s">
+        <v>1926</v>
+      </c>
+      <c r="C489" s="24">
+        <v>45334</v>
+      </c>
+      <c r="D489" s="22" t="s">
+        <v>1931</v>
+      </c>
+      <c r="E489" s="22">
+        <v>743506</v>
+      </c>
+      <c r="F489" s="22" t="s">
+        <v>350</v>
+      </c>
+      <c r="G489" s="24">
+        <v>45335</v>
+      </c>
+      <c r="H489" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I489" s="23" t="s">
         <v>1803</v>
       </c>
-      <c r="E488" s="22">
-        <v>55555</v>
-      </c>
-      <c r="I488" s="23" t="s">
-        <v>1804</v>
-      </c>
-      <c r="J488" s="21" t="s">
-        <v>1803</v>
-      </c>
-      <c r="K488" s="22" t="s">
-        <v>1933</v>
-      </c>
-      <c r="M488" s="22" t="s">
+      <c r="J489" s="21" t="s">
+        <v>1931</v>
+      </c>
+      <c r="K489" s="22" t="s">
+        <v>1932</v>
+      </c>
+      <c r="M489" s="22" t="s">
         <v>147</v>
       </c>
     </row>
@@ -30823,7 +30844,7 @@
   <conditionalFormatting sqref="D4:D28 D30:D32 D34:D159">
     <cfRule type="duplicateValues" dxfId="39" priority="37"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D488:D1048576 D375 D165:D206 D211 D213:D298 D343:D344 D377:D486">
+  <conditionalFormatting sqref="D375 D165:D206 D211 D213:D298 D343:D344 D377:D486 D488:D1048576">
     <cfRule type="duplicateValues" dxfId="39" priority="99"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E160">
@@ -30831,8 +30852,8 @@
     <cfRule type="duplicateValues" dxfId="39" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E165:E298 E1:E3 E343:E344 E375:E1048576">
+    <cfRule type="duplicateValues" dxfId="39" priority="91"/>
     <cfRule type="duplicateValues" dxfId="39" priority="90"/>
-    <cfRule type="duplicateValues" dxfId="39" priority="91"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
     <cfRule type="duplicateValues" dxfId="39" priority="74"/>
@@ -30922,7 +30943,7 @@
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;12&amp;K0078D7 OFFICIAL </oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -30933,7 +30954,7 @@
       <selection sqref="A1:A78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
@@ -30943,6 +30964,33 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="691f3940-da01-4610-8a13-7e6f036c2548" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="74dbb798-63e8-4411-94d7-398665c805e3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="691f3940-da01-4610-8a13-7e6f036c2548">
+      <UserInfo>
+        <DisplayName>Odunayo Olufemi</DisplayName>
+        <AccountId>340</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010035F00B5F6B81D145829BBB93F2043D07" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c024d4678e8ddd8c8a664f05a2d02ad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="74dbb798-63e8-4411-94d7-398665c805e3" xmlns:ns3="691f3940-da01-4610-8a13-7e6f036c2548" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ee14520912c247aa9ad2f1820187504a" ns2:_="" ns3:_="">
     <xsd:import namespace="74dbb798-63e8-4411-94d7-398665c805e3"/>
@@ -31197,34 +31245,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4FD4AE5-A275-4710-96E6-3074C94F50BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="691f3940-da01-4610-8a13-7e6f036c2548"/>
+    <ds:schemaRef ds:uri="74dbb798-63e8-4411-94d7-398665c805e3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="691f3940-da01-4610-8a13-7e6f036c2548" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="74dbb798-63e8-4411-94d7-398665c805e3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="691f3940-da01-4610-8a13-7e6f036c2548">
-      <UserInfo>
-        <DisplayName>Odunayo Olufemi</DisplayName>
-        <AccountId>340</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD201087-7430-4DBC-91FB-E5375E0F53E1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20E6ECBA-E825-4808-AC15-32F716C0C131}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -31241,23 +31281,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD201087-7430-4DBC-91FB-E5375E0F53E1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4FD4AE5-A275-4710-96E6-3074C94F50BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="691f3940-da01-4610-8a13-7e6f036c2548"/>
-    <ds:schemaRef ds:uri="74dbb798-63e8-4411-94d7-398665c805e3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Change to ignore brackets in address
</commit_message>
<xml_diff>
--- a/LandRegistryProject/TestDatas/TittleNumer.xlsx
+++ b/LandRegistryProject/TestDatas/TittleNumer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amos.Awaghade\source\repos\LandRegistryBulk-Discharge-Automation\LandRegistryProject\TestDatas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6333AA5-45F0-491B-811A-A21B03028194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B46BD15-A8D0-4F5A-9C22-A3D921DF8168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{400498CB-F334-4E68-B062-A427E2481F8E}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1933" uniqueCount="1933">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1934" uniqueCount="1934">
   <si>
     <t>Daily Download</t>
   </si>
@@ -5845,7 +5845,10 @@
     <t>31 Wallace Green Way, Walkern, Stevenage (SG2 7FB)</t>
   </si>
   <si>
-    <t>HD602384/L099LHT/221</t>
+    <t>31 Wallace Green Way, Walkern, Stevenage SG2 7FB</t>
+  </si>
+  <si>
+    <t>HD602384/M182MHT/221</t>
   </si>
 </sst>
 </file>
@@ -6912,7 +6915,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>190500</xdr:colOff>
       <xdr:row>3036</xdr:row>
       <xdr:rowOff>160602</xdr:rowOff>
     </xdr:to>
@@ -7307,7 +7310,7 @@
   <dimension ref="A1:R489"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A450" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K488" sqref="K488"/>
+      <selection activeCell="J489" sqref="J489:M489"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
@@ -7328,8 +7331,8 @@
     <col min="15" max="15" width="14.42578125" customWidth="1" style="24"/>
     <col min="16" max="16" width="9.140625" customWidth="1" style="22"/>
     <col min="17" max="17" width="59" customWidth="1" style="22"/>
-    <col min="18" max="24" width="9.140625" customWidth="1" style="22"/>
-    <col min="25" max="16384" width="9.140625" customWidth="1" style="22"/>
+    <col min="18" max="25" width="9.140625" customWidth="1" style="22"/>
+    <col min="26" max="16384" width="9.140625" customWidth="1" style="22"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1" s="6" customFormat="1">
@@ -30801,7 +30804,7 @@
         <v>45334</v>
       </c>
       <c r="D489" s="22" t="s">
-        <v>1931</v>
+        <v>1932</v>
       </c>
       <c r="E489" s="22">
         <v>743506</v>
@@ -30822,7 +30825,7 @@
         <v>1931</v>
       </c>
       <c r="K489" s="22" t="s">
-        <v>1932</v>
+        <v>1933</v>
       </c>
       <c r="M489" s="22" t="s">
         <v>147</v>
@@ -30964,33 +30967,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="691f3940-da01-4610-8a13-7e6f036c2548" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="74dbb798-63e8-4411-94d7-398665c805e3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="691f3940-da01-4610-8a13-7e6f036c2548">
-      <UserInfo>
-        <DisplayName>Odunayo Olufemi</DisplayName>
-        <AccountId>340</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010035F00B5F6B81D145829BBB93F2043D07" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c024d4678e8ddd8c8a664f05a2d02ad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="74dbb798-63e8-4411-94d7-398665c805e3" xmlns:ns3="691f3940-da01-4610-8a13-7e6f036c2548" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ee14520912c247aa9ad2f1820187504a" ns2:_="" ns3:_="">
     <xsd:import namespace="74dbb798-63e8-4411-94d7-398665c805e3"/>
@@ -31245,26 +31221,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4FD4AE5-A275-4710-96E6-3074C94F50BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="691f3940-da01-4610-8a13-7e6f036c2548"/>
-    <ds:schemaRef ds:uri="74dbb798-63e8-4411-94d7-398665c805e3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD201087-7430-4DBC-91FB-E5375E0F53E1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="691f3940-da01-4610-8a13-7e6f036c2548" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="74dbb798-63e8-4411-94d7-398665c805e3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="691f3940-da01-4610-8a13-7e6f036c2548">
+      <UserInfo>
+        <DisplayName>Odunayo Olufemi</DisplayName>
+        <AccountId>340</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20E6ECBA-E825-4808-AC15-32F716C0C131}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -31281,4 +31265,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD201087-7430-4DBC-91FB-E5375E0F53E1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4FD4AE5-A275-4710-96E6-3074C94F50BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="691f3940-da01-4610-8a13-7e6f036c2548"/>
+    <ds:schemaRef ds:uri="74dbb798-63e8-4411-94d7-398665c805e3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>